<commit_message>
Desafio 09 - Termiando OK solo falta Mendoza pero esta mal hecho
</commit_message>
<xml_diff>
--- a/Desafios/09/Pair Programming.xlsx
+++ b/Desafios/09/Pair Programming.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\desarrollo\Bootcamp 71241\Desafios\09\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\AppData\Development\Bootcamp-71241\Desafios\09\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F546316-1DC8-48FD-ABDA-99DCBB7F3855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A18F9F3-8025-4CE6-A117-00BC7E281E51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>Grupos</t>
   </si>
@@ -139,13 +139,16 @@
   </si>
   <si>
     <t>Tareas de Pair Programming - Práctico 09</t>
+  </si>
+  <si>
+    <t>OK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -185,7 +188,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,12 +210,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEA9999"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -314,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -341,6 +338,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -350,29 +365,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -776,30 +770,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:D26"/>
+  <dimension ref="B3:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:D14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
     <col min="2" max="2" width="14" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="28.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="19"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:4" ht="49.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="10" t="s">
+    <row r="3" spans="2:5" ht="15.75" thickBot="1"/>
+    <row r="4" spans="2:5" ht="49.15" customHeight="1" thickBot="1">
+      <c r="B4" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
-    </row>
-    <row r="5" spans="2:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="17"/>
+      <c r="D4" s="18"/>
+    </row>
+    <row r="5" spans="2:5" ht="40.5" customHeight="1" thickBot="1">
       <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
@@ -810,84 +805,102 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="13">
+    <row r="6" spans="2:5" ht="40.5" customHeight="1" thickBot="1">
+      <c r="B6" s="10">
         <v>1</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="11" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="15">
+      <c r="E6" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="40.5" customHeight="1" thickBot="1">
+      <c r="B7" s="10">
         <v>2</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="11" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="13">
+      <c r="E7" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="40.5" customHeight="1" thickBot="1">
+      <c r="B8" s="10">
         <v>3</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="15">
+      <c r="E8" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="40.5" customHeight="1" thickBot="1">
+      <c r="B9" s="10">
         <v>4</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="15">
+      <c r="E9" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="40.5" customHeight="1" thickBot="1">
+      <c r="B10" s="10">
         <v>5</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="17">
+      <c r="E10" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="40.5" customHeight="1" thickBot="1">
+      <c r="B11" s="10">
         <v>6</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="11" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="13">
+      <c r="E11" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="40.5" customHeight="1" thickBot="1">
+      <c r="B12" s="12">
         <v>7</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:5" ht="40.5" customHeight="1" thickBot="1">
       <c r="B13" s="4">
         <v>8</v>
       </c>
@@ -898,18 +911,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="19">
+    <row r="14" spans="2:5" ht="40.5" customHeight="1" thickBot="1">
+      <c r="B14" s="14">
         <v>9</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="15" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E14" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="40.5" customHeight="1" thickBot="1">
       <c r="B15" s="4">
         <v>10</v>
       </c>
@@ -920,7 +936,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:5" ht="40.5" customHeight="1" thickBot="1">
       <c r="B16" s="4">
         <v>11</v>
       </c>
@@ -931,40 +947,49 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="15">
+    <row r="17" spans="2:5" ht="40.5" customHeight="1" thickBot="1">
+      <c r="B17" s="10">
         <v>12</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="15">
+      <c r="E17" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="40.5" customHeight="1" thickBot="1">
+      <c r="B18" s="10">
         <v>13</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="15">
+      <c r="E18" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="40.5" customHeight="1" thickBot="1">
+      <c r="B19" s="10">
         <v>14</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="11" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E19" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="40.5" customHeight="1" thickBot="1">
       <c r="B20" s="4">
         <v>15</v>
       </c>
@@ -975,7 +1000,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" ht="40.5" customHeight="1" thickBot="1">
       <c r="B21" s="4">
         <v>16</v>
       </c>
@@ -986,7 +1011,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" ht="40.5" customHeight="1" thickBot="1">
       <c r="B22" s="4">
         <v>17</v>
       </c>
@@ -997,28 +1022,28 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" ht="40.5" customHeight="1" thickBot="1">
       <c r="B23" s="4">
         <v>18</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="2:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" ht="40.5" customHeight="1" thickBot="1">
       <c r="B24" s="4">
         <v>19</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="2:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" ht="40.5" customHeight="1" thickBot="1">
       <c r="B25" s="4">
         <v>20</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="2:4" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" ht="40.5" customHeight="1" thickBot="1">
       <c r="B26" s="9"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>

</xml_diff>

<commit_message>
Correccion faltante 09 - Vera, Bonader y Diaz Perdomo TERMINADO OK
</commit_message>
<xml_diff>
--- a/Desafios/09/Pair Programming.xlsx
+++ b/Desafios/09/Pair Programming.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\AppData\Development\Bootcamp-71241\Desafios\09\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A18F9F3-8025-4CE6-A117-00BC7E281E51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1CFA96-1F1A-45DA-8711-08AFAED30A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>Grupos</t>
   </si>
@@ -356,17 +356,17 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -773,7 +773,7 @@
   <dimension ref="B3:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -782,17 +782,17 @@
     <col min="2" max="2" width="14" style="1" customWidth="1"/>
     <col min="3" max="3" width="28.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="28.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="19"/>
+    <col min="5" max="5" width="8.85546875" style="16"/>
     <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="15.75" thickBot="1"/>
     <row r="4" spans="2:5" ht="49.15" customHeight="1" thickBot="1">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="19"/>
     </row>
     <row r="5" spans="2:5" ht="40.5" customHeight="1" thickBot="1">
       <c r="B5" s="2" t="s">
@@ -815,7 +815,7 @@
       <c r="D6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -829,7 +829,7 @@
       <c r="D7" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -843,7 +843,7 @@
       <c r="D8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -857,7 +857,7 @@
       <c r="D9" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -871,7 +871,7 @@
       <c r="D10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -885,7 +885,7 @@
       <c r="D11" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -921,19 +921,22 @@
       <c r="D14" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="16" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="40.5" customHeight="1" thickBot="1">
-      <c r="B15" s="4">
+      <c r="B15" s="14">
         <v>10</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="15" t="s">
         <v>8</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="40.5" customHeight="1" thickBot="1">
@@ -957,7 +960,7 @@
       <c r="D17" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -971,7 +974,7 @@
       <c r="D18" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -985,7 +988,7 @@
       <c r="D19" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1001,14 +1004,17 @@
       </c>
     </row>
     <row r="21" spans="2:5" ht="40.5" customHeight="1" thickBot="1">
-      <c r="B21" s="4">
+      <c r="B21" s="14">
         <v>16</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>14</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="40.5" customHeight="1" thickBot="1">

</xml_diff>